<commit_message>
:zap: OTIMIZAÇÃO DE ETAPAS
Esse novo código realiza a colagem em blocos conforme os nomes são copias de 4 em 4 vezes, usando a variável linha_inicial_c12 para manter o controle da posição. Depois de terminar o processo mais rápido sem deixar carteirinhas em vazio economizando folhas de impressão.
</commit_message>
<xml_diff>
--- a/Carteirinhas-V-A.xlsx
+++ b/Carteirinhas-V-A.xlsx
@@ -3655,7 +3655,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Rayssa Lorena de Souza do Amaral</t>
+          <t>Arthur Corrêa de Souza</t>
         </is>
       </c>
       <c r="N12" s="20" t="n"/>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Arthur Corrêa de Souza</t>
+          <t>Dhiarlley Santos Ramos</t>
         </is>
       </c>
       <c r="G26" s="20" t="n"/>
@@ -3862,7 +3862,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Renan Henrique da Silva Constantino</t>
+          <t>Emanuelly Vitória dos Santos Silva</t>
         </is>
       </c>
       <c r="N26" s="20" t="n"/>
@@ -4058,7 +4058,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Dhiarlley Santos Ramos</t>
+          <t>Gabriel Pereira Silva Fadeli</t>
         </is>
       </c>
       <c r="G40" s="20" t="n"/>
@@ -4069,7 +4069,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Samuel Alencar Felix</t>
+          <t>Giulia Amanayara Ribeiro Reis</t>
         </is>
       </c>
       <c r="N40" s="20" t="n"/>
@@ -4265,7 +4265,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Emanuelly Vitória dos Santos Silva</t>
+          <t>Heitor Henrique Alves Santos</t>
         </is>
       </c>
       <c r="G54" s="20" t="n"/>
@@ -4276,7 +4276,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Valentina Bispo Santana</t>
+          <t>Heitor Natanael Santos de Oliveira</t>
         </is>
       </c>
       <c r="N54" s="20" t="n"/>
@@ -4472,7 +4472,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Gabriel Pereira Silva Fadeli</t>
+          <t>Heitor Santos Aguado</t>
         </is>
       </c>
       <c r="G68" s="20" t="n"/>
@@ -4483,7 +4483,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Vinícius da Silva Nichel</t>
+          <t>Henry Lucca Alves Aguiar</t>
         </is>
       </c>
       <c r="N68" s="20" t="n"/>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Giulia Amanayara Ribeiro Reis</t>
+          <t>Jean Arthur da Silva Azevedo</t>
         </is>
       </c>
       <c r="G82" s="20" t="n"/>
@@ -4690,7 +4690,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Heitor Andrade Ferreira dos Santos</t>
+          <t>Kauâ Lucca Alves dos Santos</t>
         </is>
       </c>
       <c r="N82" s="20" t="n"/>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Heitor Henrique Alves Santos</t>
+          <t>Laryssa de Jesus Rodrigues</t>
         </is>
       </c>
       <c r="G96" s="20" t="n"/>
@@ -4897,7 +4897,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>Brenda Mikaelly Castro Pimentel</t>
+          <t>Laura Isabelly Santos Vieira</t>
         </is>
       </c>
       <c r="N96" s="20" t="n"/>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Heitor Natanael Santos de Oliveira</t>
+          <t>Lívia dos Santos Capodeferro</t>
         </is>
       </c>
       <c r="G110" s="20" t="n"/>
@@ -5104,7 +5104,7 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>Raylan Canuto Peixoto</t>
+          <t>Miguel Marçal de Oliveira</t>
         </is>
       </c>
       <c r="N110" s="20" t="n"/>
@@ -5300,13 +5300,19 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Heitor Santos Aguado</t>
+          <t>Nathan Souza Martins</t>
         </is>
       </c>
       <c r="G124" s="20" t="n"/>
       <c r="I124" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
+        </is>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>Neudismar Stephia de Los Angeles
+Cermeño Guzman</t>
         </is>
       </c>
       <c r="N124" s="20" t="n"/>
@@ -5502,13 +5508,18 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Henry Lucca Alves Aguiar</t>
+          <t>Pedro da Silva Alexandre</t>
         </is>
       </c>
       <c r="G138" s="20" t="n"/>
       <c r="I138" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>Pedro Henrique Cassiano Machado</t>
         </is>
       </c>
       <c r="N138" s="20" t="n"/>
@@ -5704,13 +5715,18 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Jean Arthur da Silva Azevedo</t>
+          <t>Rayssa Lorena de Souza do Amaral</t>
         </is>
       </c>
       <c r="G152" s="20" t="n"/>
       <c r="I152" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>Renan Henrique da Silva Constantino</t>
         </is>
       </c>
       <c r="N152" s="20" t="n"/>
@@ -5906,13 +5922,18 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Kauâ Lucca Alves dos Santos</t>
+          <t>Samuel Alencar Felix</t>
         </is>
       </c>
       <c r="G166" s="20" t="n"/>
       <c r="I166" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
+        </is>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>Valentina Bispo Santana</t>
         </is>
       </c>
       <c r="N166" s="20" t="n"/>
@@ -6108,13 +6129,18 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Laryssa de Jesus Rodrigues</t>
+          <t>Vinícius da Silva Nichel</t>
         </is>
       </c>
       <c r="G180" s="20" t="n"/>
       <c r="I180" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
+        </is>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>Heitor Andrade Ferreira dos Santos</t>
         </is>
       </c>
       <c r="N180" s="20" t="n"/>
@@ -6310,13 +6336,18 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Laura Isabelly Santos Vieira</t>
+          <t>Brenda Mikaelly Castro Pimentel</t>
         </is>
       </c>
       <c r="G194" s="20" t="n"/>
       <c r="I194" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
+        </is>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>Raylan Canuto Peixoto</t>
         </is>
       </c>
       <c r="N194" s="20" t="n"/>
@@ -6510,11 +6541,6 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
-      <c r="C208" t="inlineStr">
-        <is>
-          <t>Lívia dos Santos Capodeferro</t>
-        </is>
-      </c>
       <c r="G208" s="20" t="n"/>
       <c r="I208" s="9" t="inlineStr">
         <is>
@@ -6712,11 +6738,6 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
-      <c r="C222" t="inlineStr">
-        <is>
-          <t>Miguel Marçal de Oliveira</t>
-        </is>
-      </c>
       <c r="G222" s="20" t="n"/>
       <c r="I222" s="9" t="inlineStr">
         <is>
@@ -6914,11 +6935,6 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
-      <c r="C236" t="inlineStr">
-        <is>
-          <t>Nathan Souza Martins</t>
-        </is>
-      </c>
       <c r="G236" s="20" t="n"/>
       <c r="I236" s="9" t="inlineStr">
         <is>
@@ -7116,12 +7132,6 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
-        <is>
-          <t>Neudismar Stephia de Los Angeles
-Cermeño Guzman</t>
-        </is>
-      </c>
       <c r="G250" s="20" t="n"/>
       <c r="I250" s="9" t="inlineStr">
         <is>
@@ -7319,11 +7329,6 @@
           <t xml:space="preserve">Nome: </t>
         </is>
       </c>
-      <c r="C264" t="inlineStr">
-        <is>
-          <t>Pedro da Silva Alexandre</t>
-        </is>
-      </c>
       <c r="G264" s="20" t="n"/>
       <c r="I264" s="9" t="inlineStr">
         <is>
@@ -7519,11 +7524,6 @@
       <c r="B278" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="C278" t="inlineStr">
-        <is>
-          <t>Pedro Henrique Cassiano Machado</t>
         </is>
       </c>
       <c r="G278" s="20" t="n"/>

</xml_diff>